<commit_message>
Added the transaction adpater to the kotlin project
</commit_message>
<xml_diff>
--- a/Goals.xlsx
+++ b/Goals.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t xml:space="preserve">Projects to Make</t>
   </si>
@@ -41,6 +41,12 @@
     <t xml:space="preserve">Lift lelo</t>
   </si>
   <si>
+    <t xml:space="preserve">Skills to learn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learn HTML, CSS and JS</t>
+  </si>
+  <si>
     <t xml:space="preserve">Timeline</t>
   </si>
   <si>
@@ -59,7 +65,7 @@
     <t xml:space="preserve">Conclude the stuff borrowing app</t>
   </si>
   <si>
-    <t xml:space="preserve">Conclude Track my Stuff</t>
+    <t xml:space="preserve">Get proficiency in JS</t>
   </si>
   <si>
     <t xml:space="preserve">Features / Skill set required</t>
@@ -97,11 +103,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DDD&quot;, &quot;MMMM\ D&quot;, &quot;YYYY"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -123,12 +130,20 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -173,7 +188,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -182,7 +197,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -190,7 +209,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -211,10 +230,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:B49"/>
+  <dimension ref="A2:B54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B55" activeCellId="0" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -258,219 +277,235 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="2" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="n">
         <v>44203</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="n">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="n">
         <v>44204</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="n">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="n">
         <v>44205</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="n">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="n">
         <v>44206</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="n">
+      <c r="B19" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="n">
         <v>44207</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="n">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="n">
         <v>44208</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="n">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="n">
         <v>44209</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="n">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="n">
         <v>44210</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="n">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="n">
         <v>44211</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="n">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4" t="n">
         <v>44212</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="n">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4" t="n">
         <v>44213</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="n">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4" t="n">
         <v>44214</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="n">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4" t="n">
         <v>44215</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="n">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4" t="n">
         <v>44216</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="n">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4" t="n">
         <v>44217</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="n">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4" t="n">
         <v>44218</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="n">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4" t="n">
         <v>44219</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="n">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="4" t="n">
         <v>44220</v>
       </c>
-      <c r="B28" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="n">
+      <c r="B33" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="4" t="n">
         <v>44221</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="n">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="4" t="n">
         <v>44222</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="n">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="4" t="n">
         <v>44223</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3" t="n">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4" t="n">
         <v>44224</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3" t="n">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="4" t="n">
         <v>44225</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3" t="n">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="4" t="n">
         <v>44226</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="3" t="n">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="4" t="n">
         <v>44227</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="3" t="n">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="4" t="n">
         <v>44228</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="3" t="n">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="4" t="n">
         <v>44229</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="3" t="n">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="4" t="n">
         <v>44230</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="3" t="n">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="4" t="n">
         <v>44231</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="3" t="n">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="4" t="n">
         <v>44232</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3" t="n">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="4" t="n">
         <v>44233</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="3" t="n">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="4" t="n">
         <v>44234</v>
       </c>
-      <c r="B42" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="3" t="n">
+      <c r="B47" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="4" t="n">
         <v>44235</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="3" t="n">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="4" t="n">
         <v>44236</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="3" t="n">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="4" t="n">
         <v>44237</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="3" t="n">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="4" t="n">
         <v>44238</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="3" t="n">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="4" t="n">
         <v>44239</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="3" t="n">
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="4" t="n">
         <v>44240</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="3" t="n">
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="4" t="n">
         <v>44241</v>
       </c>
-      <c r="B49" s="0" t="s">
-        <v>12</v>
+      <c r="B54" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -503,68 +538,68 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
-        <v>18</v>
+      <c r="A11" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4"/>
+      <c r="A12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
-        <v>20</v>
+      <c r="A13" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>